<commit_message>
Removed childName from Excel
</commit_message>
<xml_diff>
--- a/migrate3.xlsx
+++ b/migrate3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B3329F-5E2A-46E6-AC74-090F0FA69E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C06B03-EF13-4275-99A3-84F1EB4FE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="60">
   <si>
     <t>resourceType</t>
   </si>
@@ -98,36 +98,24 @@
     <t>document</t>
   </si>
   <si>
-    <t>API_Save</t>
-  </si>
-  <si>
     <t>aPI_Save_t</t>
   </si>
   <si>
     <t>action</t>
   </si>
   <si>
-    <t>Last Priced</t>
-  </si>
-  <si>
     <t>lastPricedDate_t</t>
   </si>
   <si>
     <t>attribute</t>
   </si>
   <si>
-    <t>Constraint Margin Rate based on  Add Tax</t>
-  </si>
-  <si>
     <t>marginRateBasedOnFreightAndAddTax</t>
   </si>
   <si>
     <t>rule</t>
   </si>
   <si>
-    <t>Test_SR</t>
-  </si>
-  <si>
     <t>test_SR</t>
   </si>
   <si>
@@ -140,27 +128,15 @@
     <t>transactionLine</t>
   </si>
   <si>
-    <t>Back</t>
-  </si>
-  <si>
     <t>back_l</t>
   </si>
   <si>
-    <t>Document Number</t>
-  </si>
-  <si>
     <t>documentNumber_l</t>
   </si>
   <si>
-    <t>Tax Exempt Reason</t>
-  </si>
-  <si>
     <t>taxExemptReason</t>
   </si>
   <si>
-    <t>User Import</t>
-  </si>
-  <si>
     <t>oRCL_SFDC_UserImport</t>
   </si>
   <si>
@@ -203,9 +179,6 @@
     <t>UTIL_LIBRARY</t>
   </si>
   <si>
-    <t>CalculateTax</t>
-  </si>
-  <si>
     <t>calculateTax</t>
   </si>
   <si>
@@ -215,9 +188,6 @@
     <t>Paramount Quote to Order (oraclecpqo_bmClone_2)</t>
   </si>
   <si>
-    <t>Account Location Array</t>
-  </si>
-  <si>
     <t>accountLocationArray_t</t>
   </si>
   <si>
@@ -245,7 +215,7 @@
     <t>data_table</t>
   </si>
   <si>
-    <t>ExePkgSep20T1</t>
+    <t>ExePkgSep30T2</t>
   </si>
 </sst>
 </file>
@@ -640,9 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991D8937-EF2D-4E7C-A283-A813F0E97320}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -656,8 +624,8 @@
     <col min="8" max="8" width="24.85546875" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
     <col min="10" max="10" width="29.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" customWidth="1"/>
     <col min="13" max="13" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -704,22 +672,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="b">
         <v>0</v>
@@ -728,24 +696,24 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -757,18 +725,18 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -777,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -796,18 +764,18 @@
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -816,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -840,15 +808,15 @@
         <v>20</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -857,7 +825,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -878,18 +846,18 @@
         <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -898,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -919,18 +887,18 @@
         <v>19</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -939,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -960,97 +928,97 @@
         <v>19</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>0</v>
@@ -1059,18 +1027,18 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
@@ -1079,7 +1047,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -1091,27 +1059,27 @@
         <v>1</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1120,7 +1088,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -1132,27 +1100,27 @@
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1161,7 +1129,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
@@ -1173,27 +1141,27 @@
         <v>1</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -1202,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
@@ -1223,13 +1191,13 @@
         <v>19</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Transaction Name and Resource Type
</commit_message>
<xml_diff>
--- a/migrate3.xlsx
+++ b/migrate3.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C06B03-EF13-4275-99A3-84F1EB4FE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949D48D5-7CBE-485E-9537-772334F1D5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -222,16 +222,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -607,26 +601,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991D8937-EF2D-4E7C-A283-A813F0E97320}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8607365E-6211-4245-A766-79FA4CB1F6CD}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="51" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="29.5703125" customWidth="1"/>
-    <col min="11" max="11" width="34.7109375" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1201,8 +1194,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>